<commit_message>
jobshet 10 praktikum 4
</commit_message>
<xml_diff>
--- a/PWL_POS/public/template_level.xlsx
+++ b/PWL_POS/public/template_level.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_25\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8E5F21-3895-46CE-938F-758137063956}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B4110D-00E4-4181-9C50-8926DAA33AF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{EADA77FB-A402-4B8A-81F9-A3A5091F62AF}"/>
   </bookViews>
@@ -39,10 +39,10 @@
     <t>level_nama</t>
   </si>
   <si>
-    <t>CTM</t>
+    <t>SPV</t>
   </si>
   <si>
-    <t>Customer</t>
+    <t>Supervisor</t>
   </si>
 </sst>
 </file>
@@ -406,7 +406,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>